<commit_message>
11th commit : 발표후 피드백 - graph_legend
</commit_message>
<xml_diff>
--- a/hs_meta.xlsx
+++ b/hs_meta.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="최근 0일 서버의 랭크" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="최근 7일 REGION_KR서버의 DIAMOND랭크" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Matchups" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,22 +457,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Plague Death Knight</t>
+          <t>부정 죽음의 기사</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>55.9%</t>
+          <t>28.8%</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>6.8%</t>
+          <t>7.3%</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>120,000</t>
+          <t>35,000</t>
         </is>
       </c>
     </row>
@@ -484,22 +484,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>부정 죽음의 기사</t>
+          <t>Plague Death Knight</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>39.7%</t>
+          <t>53.5%</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>3.8%</t>
+          <t>5.8%</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>71,000</t>
+          <t>27,000</t>
         </is>
       </c>
     </row>
@@ -516,7 +516,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>41.1%</t>
+          <t>50.4%</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -526,7 +526,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>43,000</t>
+          <t>11,000</t>
         </is>
       </c>
     </row>
@@ -538,22 +538,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>냉기 죽음의 기사</t>
+          <t>Highlander Blood Death Knight</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>48.0%</t>
+          <t>50.5%</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.0%</t>
+          <t>0.6%</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>19,000</t>
+          <t>2,800</t>
         </is>
       </c>
     </row>
@@ -570,7 +570,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>48.4%</t>
+          <t>45.2%</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -580,7 +580,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>12,000</t>
+          <t>2,600</t>
         </is>
       </c>
     </row>
@@ -592,12 +592,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Highlander Blood Death Knight</t>
+          <t>냉기 죽음의 기사</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>55.7%</t>
+          <t>46.5%</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -607,7 +607,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>6,500</t>
+          <t>1,700</t>
         </is>
       </c>
     </row>
@@ -624,17 +624,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>46.2%</t>
+          <t>46.6%</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.3%</t>
+          <t>0.6%</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>25,000</t>
+          <t>3,100</t>
         </is>
       </c>
     </row>
@@ -651,17 +651,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>56.0%</t>
+          <t>56.3%</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2.5%</t>
+          <t>5.0%</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>47,000</t>
+          <t>24,000</t>
         </is>
       </c>
     </row>
@@ -673,22 +673,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>빅 악마사냥꾼</t>
+          <t>하이랜더 악마사냥꾼</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>36.6%</t>
+          <t>43.5%</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.3%</t>
+          <t>0.1%</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>5,300</t>
+          <t>550</t>
         </is>
       </c>
     </row>
@@ -700,22 +700,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>하이랜더 악마사냥꾼</t>
+          <t>유물 악마사냥꾼</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>43.2%</t>
+          <t>40.7%</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.2%</t>
+          <t>0.08%</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>4,100</t>
+          <t>370</t>
         </is>
       </c>
     </row>
@@ -727,22 +727,22 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>유물 악마사냥꾼</t>
+          <t>빅 악마사냥꾼</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>38.6%</t>
+          <t>48.9%</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.2%</t>
+          <t>0.06%</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>3,500</t>
+          <t>300</t>
         </is>
       </c>
     </row>
@@ -759,17 +759,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>24.0%</t>
+          <t>32.6%</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.4%</t>
+          <t>0.10%</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>7,400</t>
+          <t>470</t>
         </is>
       </c>
     </row>
@@ -786,17 +786,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>61.0%</t>
+          <t>54.8%</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>6.7%</t>
+          <t>5.8%</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>120,000</t>
+          <t>27,000</t>
         </is>
       </c>
     </row>
@@ -813,17 +813,17 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>58.1%</t>
+          <t>52.6%</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>3.7%</t>
+          <t>4.7%</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>70,000</t>
+          <t>22,000</t>
         </is>
       </c>
     </row>
@@ -840,17 +840,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>59.3%</t>
+          <t>53.3%</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.2%</t>
+          <t>0.6%</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>23,000</t>
+          <t>2,600</t>
         </is>
       </c>
     </row>
@@ -867,17 +867,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>37.8%</t>
+          <t>36.1%</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.2%</t>
+          <t>0.7%</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>22,000</t>
+          <t>3,400</t>
         </is>
       </c>
     </row>
@@ -894,17 +894,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>60.1%</t>
+          <t>57.0%</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>3.3%</t>
+          <t>3.7%</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>62,000</t>
+          <t>17,000</t>
         </is>
       </c>
     </row>
@@ -916,22 +916,22 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>비전 사냥꾼</t>
+          <t>하이랜더 사냥꾼</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>58.4%</t>
+          <t>57.7%</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.3%</t>
+          <t>0.8%</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>24,000</t>
+          <t>3,700</t>
         </is>
       </c>
     </row>
@@ -943,22 +943,22 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>하이랜더 사냥꾼</t>
+          <t>비전 사냥꾼</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>58.8%</t>
+          <t>57.3%</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.8%</t>
+          <t>0.6%</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>15,000</t>
+          <t>2,600</t>
         </is>
       </c>
     </row>
@@ -975,17 +975,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>45.8%</t>
+          <t>43.6%</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.5%</t>
+          <t>0.3%</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>27,000</t>
+          <t>1,500</t>
         </is>
       </c>
     </row>
@@ -1002,17 +1002,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>56.3%</t>
+          <t>55.2%</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2.5%</t>
+          <t>5.1%</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>47,000</t>
+          <t>24,000</t>
         </is>
       </c>
     </row>
@@ -1029,17 +1029,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>50.9%</t>
+          <t>51.3%</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2.1%</t>
+          <t>3.1%</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>39,000</t>
+          <t>15,000</t>
         </is>
       </c>
     </row>
@@ -1056,17 +1056,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>60.6%</t>
+          <t>54.8%</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1.8%</t>
+          <t>1.0%</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>33,000</t>
+          <t>4,800</t>
         </is>
       </c>
     </row>
@@ -1083,17 +1083,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>47.9%</t>
+          <t>48.8%</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>1.0%</t>
+          <t>0.4%</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>18,000</t>
+          <t>2,100</t>
         </is>
       </c>
     </row>
@@ -1110,17 +1110,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>47.5%</t>
+          <t>46.0%</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0.5%</t>
+          <t>0.2%</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>9,500</t>
+          <t>860</t>
         </is>
       </c>
     </row>
@@ -1137,7 +1137,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>40.6%</t>
+          <t>44.3%</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1147,7 +1147,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>3,600</t>
+          <t>800</t>
         </is>
       </c>
     </row>
@@ -1159,76 +1159,76 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Lightshow Mage</t>
+          <t>기타</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>41.9%</t>
+          <t>36.9%</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0.2%</t>
+          <t>0.6%</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>3,400</t>
+          <t>3,000</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>마법사</t>
+          <t>성기사</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>기계 마법사</t>
+          <t>어그로 성기사</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>52.1%</t>
+          <t>59.4%</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.2%</t>
+          <t>6.9%</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>3,400</t>
+          <t>33,000</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>마법사</t>
+          <t>성기사</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>기타</t>
+          <t>Showdown Paladin</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>26.0%</t>
+          <t>59.3%</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.8%</t>
+          <t>6.4%</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>34,000</t>
+          <t>30,000</t>
         </is>
       </c>
     </row>
@@ -1240,22 +1240,22 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>어그로 성기사</t>
+          <t>하이랜더 성기사</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>67.6%</t>
+          <t>54.7%</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>6.1%</t>
+          <t>2.6%</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>110,000</t>
+          <t>12,000</t>
         </is>
       </c>
     </row>
@@ -1267,22 +1267,22 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Showdown Paladin</t>
+          <t>신병 성기사</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>66.1%</t>
+          <t>49.8%</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2.9%</t>
+          <t>0.3%</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>54,000</t>
+          <t>1,600</t>
         </is>
       </c>
     </row>
@@ -1294,22 +1294,22 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>하이랜더 성기사</t>
+          <t>Earthen Paladin</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>60.7%</t>
+          <t>53.2%</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1.9%</t>
+          <t>0.3%</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>35,000</t>
+          <t>1,500</t>
         </is>
       </c>
     </row>
@@ -1321,76 +1321,76 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>신병 성기사</t>
+          <t>기타</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>54.0%</t>
+          <t>43.9%</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.8%</t>
+          <t>1.0%</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>14,000</t>
+          <t>4,900</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>성기사</t>
+          <t>사제</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Earthen Paladin</t>
+          <t>컨트롤 사제</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>53.3%</t>
+          <t>48.2%</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.2%</t>
+          <t>4.8%</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>3,400</t>
+          <t>23,000</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>성기사</t>
+          <t>사제</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>기타</t>
+          <t>언데드 사제</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>46.2%</t>
+          <t>51.1%</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2.5%</t>
+          <t>1.0%</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>46,000</t>
+          <t>4,900</t>
         </is>
       </c>
     </row>
@@ -1402,22 +1402,22 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>컨트롤 사제</t>
+          <t>하이랜더 사제</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>48.1%</t>
+          <t>46.8%</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2.2%</t>
+          <t>0.7%</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>42,000</t>
+          <t>3,300</t>
         </is>
       </c>
     </row>
@@ -1429,22 +1429,22 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>언데드 사제</t>
+          <t>Automaton Priest</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>56.4%</t>
+          <t>43.7%</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2.2%</t>
+          <t>0.2%</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>41,000</t>
+          <t>850</t>
         </is>
       </c>
     </row>
@@ -1456,22 +1456,22 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>하이랜더 사제</t>
+          <t>Ogre Priest</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>49.9%</t>
+          <t>45.6%</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>0.8%</t>
+          <t>0.08%</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>14,000</t>
+          <t>410</t>
         </is>
       </c>
     </row>
@@ -1483,76 +1483,76 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Automaton Priest</t>
+          <t>기타</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>48.5%</t>
+          <t>44.3%</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>0.5%</t>
+          <t>0.4%</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>9,100</t>
+          <t>2,100</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>사제</t>
+          <t>도적</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Ogre Priest</t>
+          <t>Wishing Rogue</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>47.3%</t>
+          <t>43.5%</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>0.2%</t>
+          <t>1.0%</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>3,200</t>
+          <t>4,800</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>사제</t>
+          <t>도적</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>기타</t>
+          <t>Mining Rogue</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>34.3%</t>
+          <t>40.4%</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>0.8%</t>
+          <t>0.7%</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>14,000</t>
+          <t>3,400</t>
         </is>
       </c>
     </row>
@@ -1564,22 +1564,22 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Mining Rogue</t>
+          <t>Ogre Rogue</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>44.2%</t>
+          <t>47.2%</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.4%</t>
+          <t>0.6%</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>26,000</t>
+          <t>3,000</t>
         </is>
       </c>
     </row>
@@ -1591,22 +1591,22 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Wishing Rogue</t>
+          <t>Mech Rogue</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>44.5%</t>
+          <t>56.4%</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1.1%</t>
+          <t>0.6%</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>20,000</t>
+          <t>2,800</t>
         </is>
       </c>
     </row>
@@ -1618,22 +1618,22 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Mech Rogue</t>
+          <t>미라클 도적</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>57.5%</t>
+          <t>49.1%</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1.0%</t>
+          <t>0.4%</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>18,000</t>
+          <t>1,600</t>
         </is>
       </c>
     </row>
@@ -1645,22 +1645,22 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Ogre Rogue</t>
+          <t>Big Rogue</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>51.3%</t>
+          <t>49.4%</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>0.9%</t>
+          <t>0.2%</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>17,000</t>
+          <t>1,100</t>
         </is>
       </c>
     </row>
@@ -1672,22 +1672,22 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Big Rogue</t>
+          <t>비밀 도적</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>57.7%</t>
+          <t>44.0%</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0.3%</t>
+          <t>0.1%</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>6,500</t>
+          <t>530</t>
         </is>
       </c>
     </row>
@@ -1699,76 +1699,76 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>미라클 도적</t>
+          <t>기타</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>47.8%</t>
+          <t>41.1%</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>0.3%</t>
+          <t>0.8%</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>6,300</t>
+          <t>3,900</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>도적</t>
+          <t>주술사</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>비밀 도적</t>
+          <t>하이랜더 주술사</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>44.3%</t>
+          <t>57.3%</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0.2%</t>
+          <t>3.4%</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>3,900</t>
+          <t>16,000</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>도적</t>
+          <t>주술사</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>기타</t>
+          <t>토템 주술사</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>35.1%</t>
+          <t>43.9%</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>1.2%</t>
+          <t>0.5%</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>23,000</t>
+          <t>2,500</t>
         </is>
       </c>
     </row>
@@ -1780,22 +1780,22 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>하이랜더 주술사</t>
+          <t>정령 주술사</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>60.3%</t>
+          <t>47.2%</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2.0%</t>
+          <t>0.3%</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>37,000</t>
+          <t>1,500</t>
         </is>
       </c>
     </row>
@@ -1807,22 +1807,22 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>토템 주술사</t>
+          <t>자연 주술사</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>57.8%</t>
+          <t>47.8%</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>0.9%</t>
+          <t>0.2%</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>16,000</t>
+          <t>780</t>
         </is>
       </c>
     </row>
@@ -1834,76 +1834,76 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>정령 주술사</t>
+          <t>기타</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>53.0%</t>
+          <t>37.4%</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0.8%</t>
+          <t>0.2%</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>15,000</t>
+          <t>1,100</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>주술사</t>
+          <t>흑마법사</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>자연 주술사</t>
+          <t>Mining Warlock</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>42.7%</t>
+          <t>51.0%</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>0.3%</t>
+          <t>3.7%</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>5,700</t>
+          <t>17,000</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>주술사</t>
+          <t>흑마법사</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>기타</t>
+          <t>저주 흑마법사</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>35.9%</t>
+          <t>47.5%</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>0.9%</t>
+          <t>1.0%</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>17,000</t>
+          <t>4,800</t>
         </is>
       </c>
     </row>
@@ -1915,22 +1915,22 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Mining Warlock</t>
+          <t>타디우스 흑마법사</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>57.0%</t>
+          <t>51.6%</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>3.9%</t>
+          <t>0.6%</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>74,000</t>
+          <t>2,900</t>
         </is>
       </c>
     </row>
@@ -1942,22 +1942,22 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>타디우스 흑마법사</t>
+          <t>하이랜더 흑마법사</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>53.1%</t>
+          <t>45.8%</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>1.1%</t>
+          <t>0.6%</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>20,000</t>
+          <t>2,800</t>
         </is>
       </c>
     </row>
@@ -1969,22 +1969,22 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>저주 흑마법사</t>
+          <t>Sludge Warlock</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>49.5%</t>
+          <t>44.5%</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>0.9%</t>
+          <t>0.5%</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>16,000</t>
+          <t>2,400</t>
         </is>
       </c>
     </row>
@@ -1996,76 +1996,76 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Sludge Warlock</t>
+          <t>기타</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>43.8%</t>
+          <t>44.9%</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.7%</t>
+          <t>0.9%</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>13,000</t>
+          <t>4,100</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>흑마법사</t>
+          <t>전사</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>하이랜더 흑마법사</t>
+          <t>컨트롤 전사</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>48.4%</t>
+          <t>51.8%</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0.3%</t>
+          <t>5.1%</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>5,900</t>
+          <t>24,000</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>흑마법사</t>
+          <t>전사</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>기타</t>
+          <t>격노 전사</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>41.6%</t>
+          <t>57.3%</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>1.6%</t>
+          <t>1.3%</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>30,000</t>
+          <t>6,300</t>
         </is>
       </c>
     </row>
@@ -2077,22 +2077,22 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>컨트롤 전사</t>
+          <t>하이랜더 전사</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>54.2%</t>
+          <t>47.9%</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>5.3%</t>
+          <t>0.6%</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>100,000</t>
+          <t>2,800</t>
         </is>
       </c>
     </row>
@@ -2104,22 +2104,22 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>격노 전사</t>
+          <t>Rock 'n' Roll Warrior</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>59.3%</t>
+          <t>49.2%</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>1.2%</t>
+          <t>0.3%</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>22,000</t>
+          <t>1,400</t>
         </is>
       </c>
     </row>
@@ -2136,17 +2136,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>45.5%</t>
+          <t>39.7%</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>0.6%</t>
+          <t>0.2%</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>11,000</t>
+          <t>790</t>
         </is>
       </c>
     </row>
@@ -2158,76 +2158,22 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>하이랜더 전사</t>
+          <t>기타</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>44.9%</t>
+          <t>44.7%</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>0.4%</t>
+          <t>0.5%</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>7,300</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>전사</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>Rock 'n' Roll Warrior</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>49.0%</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>0.4%</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>6,900</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>전사</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>기타</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>34.5%</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>1.6%</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>31,000</t>
+          <t>2,300</t>
         </is>
       </c>
     </row>
@@ -2254,68 +2200,72 @@
       <c r="A1" t="inlineStr"/>
       <c r="B1" t="inlineStr">
         <is>
+          <t>부정 죽음의 기사</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>어그로 성기사</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Showdown Paladin</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>용 드루이드</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>Plague Death Knight</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>용 드루이드</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>어그로 성기사</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Rainbow Mage</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
         <is>
           <t>컨트롤 전사</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>어그로 악마사냥꾼</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>컨트롤 사제</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>하이랜더 드루이드</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
         <is>
           <t>Mining Warlock</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>부정 죽음의 기사</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>하이랜더 드루이드</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>사냥개 사냥꾼</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Showdown Paladin</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>Rainbow Mage</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>어그로 악마사냥꾼</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr"/>
       <c r="N1" t="inlineStr">
         <is>
-          <t>혈기 죽음의 기사</t>
+          <t>하이랜더 주술사</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>컨트롤 사제</t>
+          <t>Mining Mage</t>
         </is>
       </c>
       <c r="P1" t="inlineStr"/>
@@ -2332,1087 +2282,1091 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>부정 죽음의 기사</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>부정 죽음의 기사
+Mirror matchup</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>32.26%</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>18.25%</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>20.00%</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>29.33%</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>23.44%</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>23.92%</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>39.01%</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>27.65%</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>24.72%</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>26.76%</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>25.00%</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>16.99%</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>30.13%</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>어그로 성기사</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>67.73%</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>어그로 성기사
+Mirror matchup</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>41.40%</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>70.13%</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>57.91%</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>50.20%</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>58.10%</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>47.13%</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>62.92%</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>70.28%</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>61.14%</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>64.89%</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>53.01%</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>52.38%</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Showdown Paladin</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>81.74%</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>58.59%</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Showdown Paladin
+Mirror matchup</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>67.59%</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>54.65%</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>49.06%</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>47.98%</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>59.40%</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>52.36%</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>64.16%</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>54.00%</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>65.03%</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>48.76%</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>54.55%</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>용 드루이드</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>79.99%</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>29.86%</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>32.40%</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>용 드루이드
+Mirror matchup</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>54.20%</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>53.72%</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>58.37%</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>54.25%</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>48.37%</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>50.94%</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>60.99%</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>43.70%</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>45.56%</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>64.40%</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>Plague Death Knight</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>70.66%</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>42.08%</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>45.34%</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>45.79%</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
         <is>
           <t>Plague Death Knight
 Mirror matchup</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>40.86%</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>37.32%</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>56.96%</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>46.71%</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>63.70%</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>60.74%</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>39.94%</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>39.38%</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>48.27%</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>50.30%</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>61.38%</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>64.36%</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>65.60%</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>용 드루이드</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>59.13%</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>용 드루이드
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>45.72%</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>58.61%</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>47.26%</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>61.32%</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>55.55%</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>46.96%</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>32.25%</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>61.12%</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>47.92%</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Rainbow Mage</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>76.55%</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>49.79%</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>50.86%</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>46.27%</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>54.27%</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Rainbow Mage
 Mirror matchup</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>30.84%</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>58.25%</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>57.02%</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>76.39%</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>49.89%</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>51.50%</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>30.14%</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>59.99%</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>61.19%</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>63.34%</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>71.75%</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>54.82%</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>어그로 성기사</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>62.67%</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>69.15%</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>어그로 성기사
-Mirror matchup</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>68.40%</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>62.55%</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>65.11%</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>73.66%</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>63.76%</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>44.26%</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>56.21%</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>49.85%</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>73.19%</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>74.09%</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>72.06%</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>51.56%</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>38.83%</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>64.37%</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>50.71%</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>57.72%</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>37.85%</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>52.23%</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>56.89%</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
         <is>
           <t>컨트롤 전사</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>43.03%</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>41.74%</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>31.59%</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>76.07%</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>41.89%</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>52.01%</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>41.62%</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>41.29%</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>48.43%</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
         <is>
           <t>컨트롤 전사
 Mirror matchup</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>35.95%</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>64.28%</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>35.82%</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>43.96%</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>42.48%</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>51.51%</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>48.81%</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>59.76%</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>69.32%</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>60.15%</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>51.16%</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>55.25%</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>36.73%</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>39.35%</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>42.64%</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>48.58%</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>47.13%</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>어그로 악마사냥꾼</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>60.98%</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>52.86%</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>40.59%</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>45.74%</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>52.54%</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>61.16%</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>48.83%</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>어그로 악마사냥꾼
+Mirror matchup</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>56.87%</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>61.11%</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>60.79%</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>50.19%</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>49.25%</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>56.07%</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>컨트롤 사제</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>72.34%</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>37.07%</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>47.63%</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>51.62%</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>38.67%</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>35.62%</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>44.74%</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>43.12%</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>컨트롤 사제
+Mirror matchup</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>39.88%</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>43.66%</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>41.62%</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>38.72%</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>32.39%</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>하이랜더 드루이드</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>75.27%</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>29.71%</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>35.83%</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>49.05%</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>44.44%</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>49.28%</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>63.26%</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>38.88%</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>60.11%</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>하이랜더 드루이드
+Mirror matchup</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>59.33%</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>41.26%</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>37.65%</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>62.94%</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
         <is>
           <t>Mining Warlock</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>53.28%</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>42.97%</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>37.44%</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>64.04%</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>73.23%</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>38.85%</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>45.99%</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>39.00%</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>53.03%</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>42.13%</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>60.64%</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>39.20%</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>56.33%</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>40.66%</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
         <is>
           <t>Mining Warlock
 Mirror matchup</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>65.07%</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>43.72%</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>44.91%</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>44.64%</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>51.79%</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>44.01%</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>66.10%</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>69.49%</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>62.82%</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>부정 죽음의 기사</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>36.29%</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>23.60%</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>34.88%</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>35.71%</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>34.92%</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>부정 죽음의 기사
-Mirror matchup</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>31.96%</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>30.50%</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>23.39%</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>33.06%</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>44.43%</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>47.74%</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>40.87%</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>37.20%</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>하이랜더 드루이드</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>39.25%</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>50.10%</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>26.33%</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>64.17%</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>56.27%</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>68.03%</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>하이랜더 드루이드
-Mirror matchup</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>46.90%</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>35.00%</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>58.79%</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>46.95%</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>62.60%</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>77.01%</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>67.83%</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>38.95%</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>47.05%</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>51.64%</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
         <is>
           <t>사냥개 사냥꾼</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>60.05%</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>48.49%</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>36.23%</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>56.03%</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>55.08%</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>69.49%</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>53.09%</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>75.00%</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>35.10%</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>34.96%</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>56.29%</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>67.74%</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>62.14%</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>57.35%</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>49.80%</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>58.37%</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>58.73%</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>61.04%</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
         <is>
           <t>사냥개 사냥꾼
 Mirror matchup</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>34.38%</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>58.37%</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>54.53%</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>65.04%</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>71.18%</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>60.12%</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Showdown Paladin</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>60.61%</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>69.85%</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>55.73%</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>57.51%</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>55.35%</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>76.60%</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>65.00%</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>65.61%</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>Showdown Paladin
-Mirror matchup</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>60.26%</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>59.88%</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>77.55%</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>71.53%</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>60.62%</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Rainbow Mage</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>51.72%</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>40.00%</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>43.78%</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>48.48%</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>48.20%</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>66.86%</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>41.12%</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>41.62%</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>39.73%</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>Rainbow Mage
-Mirror matchup</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>45.47%</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>65.60%</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>66.62%</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>68.66%</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>어그로 악마사냥꾼</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>49.69%</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>38.80%</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>50.14%</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>51.18%</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>55.98%</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>55.56%</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>52.95%</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>45.46%</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>40.11%</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>54.52%</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>어그로 악마사냥꾼
-Mirror matchup</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>63.10%</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>61.84%</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>55.39%</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>38.49%</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>36.65%</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>26.80%</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>40.13%</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>33.89%</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>52.25%</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>37.32%</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>34.86%</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>22.44%</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>34.39%</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>36.89%</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>기타 성기사
-Mirror matchup</t>
-        </is>
-      </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>50.38%</t>
+          <t>58.26%</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>44.35%</t>
+          <t>66.28%</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>혈기 죽음의 기사</t>
+          <t>하이랜더 주술사</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>35.63%</t>
+          <t>83.00%</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>28.24%</t>
+          <t>46.98%</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>25.90%</t>
+          <t>51.23%</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>30.67%</t>
+          <t>54.43%</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>30.50%</t>
+          <t>38.87%</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>59.12%</t>
+          <t>47.76%</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>22.98%</t>
+          <t>51.41%</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>28.81%</t>
+          <t>50.74%</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>28.46%</t>
+          <t>61.27%</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>33.37%</t>
+          <t>62.34%</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>38.15%</t>
+          <t>52.94%</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>49.50%</t>
+          <t>41.73%</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>혈기 죽음의 기사
+          <t>하이랜더 주술사
 Mirror matchup</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>40.56%</t>
+          <t>55.94%</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>컨트롤 사제</t>
+          <t>Mining Mage</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>34.39%</t>
+          <t>69.86%</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>45.17%</t>
+          <t>47.61%</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>27.93%</t>
+          <t>45.44%</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>39.84%</t>
+          <t>35.59%</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>37.17%</t>
+          <t>52.07%</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>62.79%</t>
+          <t>43.10%</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>32.16%</t>
+          <t>52.86%</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>39.87%</t>
+          <t>43.92%</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>39.37%</t>
+          <t>67.41%</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>31.33%</t>
+          <t>37.05%</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>44.60%</t>
+          <t>48.35%</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>55.64%</t>
+          <t>33.71%</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>59.43%</t>
+          <t>43.81%</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>컨트롤 사제
+          <t>Mining Mage
 Mirror matchup</t>
         </is>
       </c>

</xml_diff>

<commit_message>
13th commit : 피드백3 - data_meta 수정
</commit_message>
<xml_diff>
--- a/hs_meta.xlsx
+++ b/hs_meta.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -425,7 +425,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>기간 : LAST_PATCH, 대상 : ALL 서버의 ALL 등급 유저</t>
+          <t>기간 : LAST_PATCH, 대상 : ALL 서버의 REGION_KR 등급 유저</t>
         </is>
       </c>
     </row>
@@ -469,17 +469,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>56.2%</t>
+          <t>53.7%</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>6.8%</t>
+          <t>7.8%</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>23,000</t>
+          <t>190,000</t>
         </is>
       </c>
     </row>
@@ -491,22 +491,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>부정 죽음의 기사</t>
+          <t>혈기 죽음의 기사</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>38.9%</t>
+          <t>51.9%</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>3.9%</t>
+          <t>4.3%</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>13,000</t>
+          <t>100,000</t>
         </is>
       </c>
     </row>
@@ -518,22 +518,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>혈기 죽음의 기사</t>
+          <t>부정 죽음의 기사</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>48.2%</t>
+          <t>38.4%</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>3.3%</t>
+          <t>2.8%</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>11,000</t>
+          <t>70,000</t>
         </is>
       </c>
     </row>
@@ -550,17 +550,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>48.0%</t>
+          <t>47.0%</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.0%</t>
+          <t>0.8%</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>3,500</t>
+          <t>18,000</t>
         </is>
       </c>
     </row>
@@ -577,7 +577,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>49.6%</t>
+          <t>46.6%</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -587,7 +587,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1,900</t>
+          <t>14,000</t>
         </is>
       </c>
     </row>
@@ -604,17 +604,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>57.0%</t>
+          <t>52.4%</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.4%</t>
+          <t>0.6%</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1,100</t>
+          <t>13,000</t>
         </is>
       </c>
     </row>
@@ -631,17 +631,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>45.7%</t>
+          <t>44.6%</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.5%</t>
+          <t>1.0%</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>5,000</t>
+          <t>25,000</t>
         </is>
       </c>
     </row>
@@ -658,7 +658,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>51.6%</t>
+          <t>49.1%</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -668,7 +668,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>5,400</t>
+          <t>40,000</t>
         </is>
       </c>
     </row>
@@ -680,12 +680,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>빅 악마사냥꾼</t>
+          <t>하이랜더 악마사냥꾼</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>39.3%</t>
+          <t>41.5%</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -695,7 +695,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1,100</t>
+          <t>8,000</t>
         </is>
       </c>
     </row>
@@ -707,22 +707,22 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>하이랜더 악마사냥꾼</t>
+          <t>빅 악마사냥꾼</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>40.8%</t>
+          <t>42.8%</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.2%</t>
+          <t>0.3%</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>610</t>
+          <t>6,200</t>
         </is>
       </c>
     </row>
@@ -739,7 +739,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>36.2%</t>
+          <t>39.2%</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -749,7 +749,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>530</t>
+          <t>3,700</t>
         </is>
       </c>
     </row>
@@ -766,17 +766,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>23.9%</t>
+          <t>25.6%</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.4%</t>
+          <t>0.3%</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1,300</t>
+          <t>6,300</t>
         </is>
       </c>
     </row>
@@ -793,17 +793,17 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>61.2%</t>
+          <t>57.8%</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>6.3%</t>
+          <t>7.5%</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>21,000</t>
+          <t>190,000</t>
         </is>
       </c>
     </row>
@@ -820,17 +820,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>58.5%</t>
+          <t>54.2%</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2.7%</t>
+          <t>3.2%</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>9,200</t>
+          <t>80,000</t>
         </is>
       </c>
     </row>
@@ -847,7 +847,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>61.7%</t>
+          <t>58.9%</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -857,7 +857,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>4,400</t>
+          <t>33,000</t>
         </is>
       </c>
     </row>
@@ -874,17 +874,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>37.9%</t>
+          <t>37.3%</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.1%</t>
+          <t>0.8%</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>3,700</t>
+          <t>21,000</t>
         </is>
       </c>
     </row>
@@ -901,17 +901,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>58.2%</t>
+          <t>55.0%</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2.4%</t>
+          <t>2.3%</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>8,200</t>
+          <t>58,000</t>
         </is>
       </c>
     </row>
@@ -923,22 +923,22 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>비전 사냥꾼</t>
+          <t>하이랜더 사냥꾼</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>58.4%</t>
+          <t>59.7%</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.2%</t>
+          <t>1.7%</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>4,000</t>
+          <t>42,000</t>
         </is>
       </c>
     </row>
@@ -950,12 +950,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>하이랜더 사냥꾼</t>
+          <t>비전 사냥꾼</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>61.1%</t>
+          <t>56.0%</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -965,7 +965,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>3,400</t>
+          <t>24,000</t>
         </is>
       </c>
     </row>
@@ -982,17 +982,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>45.9%</t>
+          <t>47.5%</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.5%</t>
+          <t>1.2%</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>5,100</t>
+          <t>30,000</t>
         </is>
       </c>
     </row>
@@ -1009,17 +1009,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>58.5%</t>
+          <t>55.5%</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>4.0%</t>
+          <t>6.2%</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>13,000</t>
+          <t>150,000</t>
         </is>
       </c>
     </row>
@@ -1036,17 +1036,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>54.2%</t>
+          <t>50.9%</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>3.2%</t>
+          <t>3.4%</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>11,000</t>
+          <t>85,000</t>
         </is>
       </c>
     </row>
@@ -1063,7 +1063,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>60.3%</t>
+          <t>56.1%</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1073,7 +1073,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>7,000</t>
+          <t>50,000</t>
         </is>
       </c>
     </row>
@@ -1090,17 +1090,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>48.1%</t>
+          <t>49.4%</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0.9%</t>
+          <t>0.6%</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2,900</t>
+          <t>15,000</t>
         </is>
       </c>
     </row>
@@ -1117,17 +1117,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>51.2%</t>
+          <t>48.9%</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0.6%</t>
+          <t>0.4%</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2,000</t>
+          <t>9,500</t>
         </is>
       </c>
     </row>
@@ -1144,17 +1144,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>40.1%</t>
+          <t>38.9%</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0.2%</t>
+          <t>0.3%</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>830</t>
+          <t>6,900</t>
         </is>
       </c>
     </row>
@@ -1166,76 +1166,76 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>기계 마법사</t>
+          <t>기타</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>54.8%</t>
+          <t>30.7%</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.2%</t>
+          <t>1.1%</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>510</t>
+          <t>28,000</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>마법사</t>
+          <t>성기사</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>하이랜더 마법사</t>
+          <t>어그로 성기사</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>39.1%</t>
+          <t>59.5%</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0.1%</t>
+          <t>4.8%</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>470</t>
+          <t>120,000</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>마법사</t>
+          <t>성기사</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>기타</t>
+          <t>Showdown Paladin</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>26.9%</t>
+          <t>57.3%</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.9%</t>
+          <t>2.2%</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>6,400</t>
+          <t>55,000</t>
         </is>
       </c>
     </row>
@@ -1247,22 +1247,22 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>어그로 성기사</t>
+          <t>하이랜더 성기사</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>63.3%</t>
+          <t>54.6%</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>5.1%</t>
+          <t>1.8%</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>17,000</t>
+          <t>44,000</t>
         </is>
       </c>
     </row>
@@ -1274,22 +1274,22 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Showdown Paladin</t>
+          <t>신병 성기사</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>62.5%</t>
+          <t>53.0%</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2.7%</t>
+          <t>0.5%</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>9,400</t>
+          <t>11,000</t>
         </is>
       </c>
     </row>
@@ -1301,22 +1301,22 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>하이랜더 성기사</t>
+          <t>Earthen Paladin</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>58.6%</t>
+          <t>54.2%</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1.4%</t>
+          <t>0.3%</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>4,600</t>
+          <t>7,100</t>
         </is>
       </c>
     </row>
@@ -1328,76 +1328,76 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>신병 성기사</t>
+          <t>기타</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>54.0%</t>
+          <t>44.0%</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.8%</t>
+          <t>1.5%</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2,500</t>
+          <t>36,000</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>성기사</t>
+          <t>사제</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Earthen Paladin</t>
+          <t>컨트롤 사제</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>55.3%</t>
+          <t>47.2%</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.3%</t>
+          <t>2.4%</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1,100</t>
+          <t>61,000</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>성기사</t>
+          <t>사제</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>기타</t>
+          <t>언데드 사제</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>45.2%</t>
+          <t>54.7%</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2.2%</t>
+          <t>2.0%</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>7,500</t>
+          <t>50,000</t>
         </is>
       </c>
     </row>
@@ -1409,22 +1409,22 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>언데드 사제</t>
+          <t>하이랜더 사제</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>56.9%</t>
+          <t>47.2%</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2.6%</t>
+          <t>0.6%</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>9,000</t>
+          <t>14,000</t>
         </is>
       </c>
     </row>
@@ -1436,22 +1436,22 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>컨트롤 사제</t>
+          <t>Automaton Priest</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>48.5%</t>
+          <t>48.8%</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2.1%</t>
+          <t>0.4%</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>7,200</t>
+          <t>10,000</t>
         </is>
       </c>
     </row>
@@ -1463,22 +1463,22 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Automaton Priest</t>
+          <t>Ogre Priest</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>50.4%</t>
+          <t>47.7%</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>0.5%</t>
+          <t>0.2%</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1,800</t>
+          <t>5,100</t>
         </is>
       </c>
     </row>
@@ -1490,12 +1490,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>하이랜더 사제</t>
+          <t>기타</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>49.6%</t>
+          <t>36.7%</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1505,61 +1505,61 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1,700</t>
+          <t>13,000</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>사제</t>
+          <t>도적</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Ogre Priest</t>
+          <t>Mech Rogue</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>47.0%</t>
+          <t>57.8%</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>0.1%</t>
+          <t>1.0%</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>400</t>
+          <t>25,000</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>사제</t>
+          <t>도적</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>기타</t>
+          <t>Wishing Rogue</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>32.5%</t>
+          <t>41.9%</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>0.7%</t>
+          <t>1.0%</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2,400</t>
+          <t>24,000</t>
         </is>
       </c>
     </row>
@@ -1576,17 +1576,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>43.0%</t>
+          <t>40.7%</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1.1%</t>
+          <t>1.0%</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>3,900</t>
+          <t>24,000</t>
         </is>
       </c>
     </row>
@@ -1598,22 +1598,22 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Mech Rogue</t>
+          <t>Big Rogue</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>58.8%</t>
+          <t>48.4%</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1.0%</t>
+          <t>0.6%</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>3,300</t>
+          <t>15,000</t>
         </is>
       </c>
     </row>
@@ -1625,22 +1625,22 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Wishing Rogue</t>
+          <t>Ogre Rogue</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>47.9%</t>
+          <t>47.4%</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.0%</t>
+          <t>0.5%</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>3,200</t>
+          <t>13,000</t>
         </is>
       </c>
     </row>
@@ -1652,22 +1652,22 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Ogre Rogue</t>
+          <t>미라클 도적</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>52.9%</t>
+          <t>43.7%</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0.6%</t>
+          <t>0.5%</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2,100</t>
+          <t>12,000</t>
         </is>
       </c>
     </row>
@@ -1679,22 +1679,22 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Big Rogue</t>
+          <t>비밀 도적</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>51.3%</t>
+          <t>46.0%</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>0.4%</t>
+          <t>0.3%</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1,400</t>
+          <t>7,900</t>
         </is>
       </c>
     </row>
@@ -1706,76 +1706,76 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>미라클 도적</t>
+          <t>기타</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>46.6%</t>
+          <t>35.7%</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0.3%</t>
+          <t>0.9%</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>950</t>
+          <t>22,000</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>도적</t>
+          <t>주술사</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>비밀 도적</t>
+          <t>하이랜더 주술사</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>48.7%</t>
+          <t>56.7%</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>0.3%</t>
+          <t>4.5%</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>920</t>
+          <t>110,000</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>도적</t>
+          <t>주술사</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>기타</t>
+          <t>토템 주술사</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>35.5%</t>
+          <t>57.1%</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>1.3%</t>
+          <t>0.7%</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>4,500</t>
+          <t>17,000</t>
         </is>
       </c>
     </row>
@@ -1787,22 +1787,22 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>하이랜더 주술사</t>
+          <t>정령 주술사</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>60.7%</t>
+          <t>50.1%</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2.9%</t>
+          <t>0.5%</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>10,000</t>
+          <t>12,000</t>
         </is>
       </c>
     </row>
@@ -1814,22 +1814,22 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>토템 주술사</t>
+          <t>자연 주술사</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>59.4%</t>
+          <t>46.9%</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0.9%</t>
+          <t>0.4%</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2,900</t>
+          <t>11,000</t>
         </is>
       </c>
     </row>
@@ -1841,76 +1841,76 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>정령 주술사</t>
+          <t>기타</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>52.0%</t>
+          <t>38.4%</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>0.6%</t>
+          <t>0.7%</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>2,000</t>
+          <t>17,000</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>주술사</t>
+          <t>흑마법사</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>자연 주술사</t>
+          <t>Mining Warlock</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>45.4%</t>
+          <t>49.0%</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>0.5%</t>
+          <t>1.9%</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>1,500</t>
+          <t>48,000</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>주술사</t>
+          <t>흑마법사</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>기타</t>
+          <t>Sludge Warlock</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>37.3%</t>
+          <t>41.9%</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>1.0%</t>
+          <t>0.9%</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>3,500</t>
+          <t>22,000</t>
         </is>
       </c>
     </row>
@@ -1922,22 +1922,22 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Mining Warlock</t>
+          <t>하이랜더 흑마법사</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>53.7%</t>
+          <t>49.3%</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>2.4%</t>
+          <t>0.9%</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>8,100</t>
+          <t>22,000</t>
         </is>
       </c>
     </row>
@@ -1949,22 +1949,22 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>타디우스 흑마법사</t>
+          <t>저주 흑마법사</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>54.1%</t>
+          <t>49.0%</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>1.0%</t>
+          <t>0.8%</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>3,500</t>
+          <t>21,000</t>
         </is>
       </c>
     </row>
@@ -1976,22 +1976,22 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>저주 흑마법사</t>
+          <t>타디우스 흑마법사</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>50.5%</t>
+          <t>52.2%</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>1.0%</t>
+          <t>0.8%</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>3,200</t>
+          <t>20,000</t>
         </is>
       </c>
     </row>
@@ -2003,76 +2003,76 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Sludge Warlock</t>
+          <t>기타</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>47.3%</t>
+          <t>42.1%</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0.9%</t>
+          <t>1.2%</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>2,900</t>
+          <t>30,000</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>흑마법사</t>
+          <t>전사</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>하이랜더 흑마법사</t>
+          <t>컨트롤 전사</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>47.5%</t>
+          <t>52.4%</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>0.4%</t>
+          <t>5.4%</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>1,300</t>
+          <t>130,000</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>흑마법사</t>
+          <t>전사</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>기타</t>
+          <t>격노 전사</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>40.5%</t>
+          <t>57.4%</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>1.7%</t>
+          <t>1.8%</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>5,700</t>
+          <t>45,000</t>
         </is>
       </c>
     </row>
@@ -2084,22 +2084,22 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>컨트롤 전사</t>
+          <t>Rock 'n' Roll Warrior</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>56.5%</t>
+          <t>52.4%</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>5.8%</t>
+          <t>0.7%</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>19,000</t>
+          <t>18,000</t>
         </is>
       </c>
     </row>
@@ -2111,22 +2111,22 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>격노 전사</t>
+          <t>도발 전사</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>60.2%</t>
+          <t>44.8%</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>1.6%</t>
+          <t>0.6%</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>5,400</t>
+          <t>13,000</t>
         </is>
       </c>
     </row>
@@ -2138,22 +2138,22 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>도발 전사</t>
+          <t>하이랜더 전사</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>47.0%</t>
+          <t>47.1%</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>0.6%</t>
+          <t>0.4%</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>1,800</t>
+          <t>10,000</t>
         </is>
       </c>
     </row>
@@ -2165,76 +2165,22 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>하이랜더 전사</t>
+          <t>기타</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>48.7%</t>
+          <t>36.3%</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>0.4%</t>
+          <t>1.1%</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>1,300</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>전사</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>Rock 'n' Roll Warrior</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>50.0%</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>0.4%</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>1,300</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>전사</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>기타</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>34.8%</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>2.0%</t>
-        </is>
-      </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>6,900</t>
+          <t>28,000</t>
         </is>
       </c>
     </row>
@@ -2260,7 +2206,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>기간 : LAST_PATCH, 대상 : ALL 서버의 ALL 등급 유저</t>
+          <t>기간 : LAST_PATCH, 대상 : ALL 서버의 REGION_KR 등급 유저</t>
         </is>
       </c>
     </row>
@@ -2268,73 +2214,72 @@
       <c r="A2" t="inlineStr"/>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Plague Death Knight
-Mirror matchup</t>
+          <t>Plague Death Knight</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>42.27%</t>
+          <t>용 드루이드</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>54.35%</t>
+          <t>Rainbow Mage</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>40.99%</t>
+          <t>컨트롤 전사</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>46.99%</t>
+          <t>어그로 성기사</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>63.24%</t>
+          <t>하이랜더 주술사</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>58.80%</t>
+          <t>혈기 죽음의 기사</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>52.46%</t>
+          <t>Mining Mage</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>57.47%</t>
+          <t>하이랜더 드루이드</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>48.88%</t>
+          <t>부정 죽음의 기사</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>54.82%</t>
+          <t>컨트롤 사제</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>47.79%</t>
+          <t>사냥개 사냥꾼</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>40.92%</t>
+          <t>Showdown Paladin</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>52.95%</t>
+          <t>언데드 사제</t>
         </is>
       </c>
       <c r="P2" t="inlineStr"/>
@@ -2356,1016 +2301,1087 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>57.72%</t>
+          <t>Plague Death Knight
+Mirror matchup</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
+        <is>
+          <t>40.56%</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>44.40%</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>57.06%</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>41.95%</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>60.65%</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>53.35%</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>50.19%</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>57.87%</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>62.63%</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>60.99%</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>44.11%</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>45.60%</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>44.65%</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>용 드루이드</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>59.43%</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
         <is>
           <t>용 드루이드
 Mirror matchup</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>58.19%</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>36.02%</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>54.68%</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>78.69%</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>64.41%</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>63.58%</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>47.54%</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>37.26%</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>50.85%</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>64.72%</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>58.14%</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>63.91%</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>용 드루이드</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>45.64%</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>41.80%</t>
-        </is>
-      </c>
       <c r="D4" t="inlineStr">
+        <is>
+          <t>56.24%</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>57.58%</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>37.73%</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>46.56%</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>54.25%</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>63.54%</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>48.59%</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>78.42%</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>52.15%</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>56.14%</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>38.33%</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>64.05%</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Rainbow Mage</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>55.56%</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>43.75%</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Rainbow Mage
+Mirror matchup</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>55.50%</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>52.42%</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>51.10%</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>54.27%</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>58.08%</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>45.79%</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>71.01%</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>68.36%</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>45.73%</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>55.66%</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>52.87%</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>컨트롤 전사</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>42.93%</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>42.41%</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>44.47%</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
         <is>
           <t>컨트롤 전사
 Mirror matchup</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>38.60%</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>46.58%</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>65.62%</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>66.13%</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>49.21%</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>51.36%</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>48.50%</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>39.41%</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>56.61%</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>50.56%</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>44.16%</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>컨트롤 전사</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>59.00%</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>63.97%</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>61.39%</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>41.10%</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>50.78%</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>52.97%</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>49.81%</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>38.25%</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>67.48%</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>59.94%</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>45.37%</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>49.49%</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>56.40%</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>어그로 성기사</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>58.04%</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>62.26%</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>47.58%</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>58.89%</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
         <is>
           <t>어그로 성기사
 Mirror matchup</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>50.00%</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>60.60%</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>63.45%</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>54.30%</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>49.88%</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>40.06%</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>70.89%</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>60.00%</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>65.16%</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>57.89%</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>어그로 성기사</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>53.00%</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>45.31%</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>53.41%</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>50.00%</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Rainbow Mage
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>50.76%</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>54.75%</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>51.05%</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>67.46%</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>59.88%</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>58.33%</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>64.21%</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>43.40%</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>54.44%</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>하이랜더 주술사</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>39.34%</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>53.43%</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>48.88%</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>49.21%</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>49.21%</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>하이랜더 주술사
 Mirror matchup</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>72.27%</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>62.50%</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>58.26%</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>52.49%</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>54.82%</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>43.47%</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>49.52%</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>48.34%</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>59.91%</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Rainbow Mage</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>36.75%</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>21.30%</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>34.37%</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>39.39%</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>27.72%</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>55.19%</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>52.40%</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>61.08%</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>75.98%</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>59.33%</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>55.71%</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>57.39%</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>66.61%</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>혈기 죽음의 기사</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>46.62%</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>45.74%</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>45.69%</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>47.02%</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>45.24%</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>44.77%</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>혈기 죽음의 기사
+Mirror matchup</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>48.52%</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>44.54%</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>66.47%</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>59.98%</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>41.00%</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>53.75%</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>46.42%</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Mining Mage</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>49.77%</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>36.40%</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>41.91%</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>50.18%</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>48.94%</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>47.55%</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>51.35%</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Mining Mage
+Mirror matchup</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>36.73%</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>62.04%</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>67.55%</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>39.64%</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>49.15%</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>50.04%</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>하이랜더 드루이드</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>42.12%</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>51.40%</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>54.20%</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>61.74%</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>32.53%</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>38.87%</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>55.45%</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>63.26%</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>하이랜더 드루이드
+Mirror matchup</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>68.92%</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>61.81%</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>49.18%</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>39.05%</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>57.95%</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>부정 죽음의 기사</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>37.36%</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>21.57%</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>28.98%</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>32.51%</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>40.11%</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>24.01%</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>33.52%</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>37.95%</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>31.07%</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
         <is>
           <t>부정 죽음의 기사
 Mirror matchup</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>36.76%</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>37.83%</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>22.57%</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>25.07%</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>33.13%</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>28.26%</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>34.13%</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>31.46%</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>부정 죽음의 기사</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>41.19%</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>35.58%</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>33.86%</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>36.54%</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>37.50%</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>63.23%</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>혈기 죽음의 기사
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>35.21%</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>34.93%</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>28.50%</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>34.57%</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>컨트롤 사제</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>39.00%</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>47.84%</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>31.63%</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>40.05%</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>41.66%</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>40.66%</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>40.01%</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>32.44%</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>38.18%</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>64.78%</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>컨트롤 사제
 Mirror matchup</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>38.81%</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>38.17%</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>44.70%</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>30.76%</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>34.36%</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>35.45%</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>47.69%</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>혈기 죽음의 기사</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>47.53%</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>36.22%</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>50.78%</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>45.69%</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>41.73%</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>62.16%</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>61.18%</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>Mining Mage
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>41.41%</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>47.23%</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>46.39%</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>사냥개 사냥꾼</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>55.88%</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>43.85%</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>54.26%</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>54.62%</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>35.78%</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>44.28%</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>58.99%</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>60.35%</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>50.81%</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>65.06%</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>58.58%</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>사냥개 사냥꾼
 Mirror matchup</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>39.65%</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>45.93%</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>33.33%</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>50.71%</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>41.95%</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>55.17%</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Mining Mage</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>42.52%</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>52.45%</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>48.63%</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>50.11%</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>47.50%</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>77.42%</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>61.82%</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>60.34%</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>하이랜더 주술사
-Mirror matchup</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>59.43%</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>61.57%</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>70.23%</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>49.41%</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>57.79%</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>하이랜더 주술사</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>51.11%</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>62.73%</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>51.50%</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>59.93%</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>45.17%</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>74.92%</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>55.29%</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>54.06%</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>40.56%</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>37.70%</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>53.87%</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Showdown Paladin</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>54.39%</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>61.66%</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>44.33%</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>50.50%</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>56.59%</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>42.60%</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>46.24%</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>50.84%</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>60.94%</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>71.49%</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>52.76%</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>62.29%</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
         <is>
           <t>Showdown Paladin
 Mirror matchup</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>66.66%</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>66.66%</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>65.54%</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>55.21%</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Showdown Paladin</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>45.17%</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>49.14%</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>60.58%</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>29.10%</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>56.52%</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>66.86%</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>69.23%</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>66.66%</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>38.42%</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>33.33%</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>하이랜더 드루이드
-Mirror matchup</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>57.32%</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>48.53%</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>64.28%</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>하이랜더 드루이드</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>52.20%</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>35.27%</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>43.38%</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>40.00%</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>50.47%</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>71.73%</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>65.63%</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>49.28%</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>29.76%</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>33.33%</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>42.67%</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>56.23%</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>언데드 사제</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>55.34%</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>35.94%</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>47.12%</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>43.59%</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>45.55%</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>33.38%</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>53.57%</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>49.95%</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>42.04%</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>65.42%</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>53.60%</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>46.12%</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>43.76%</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
         <is>
           <t>언데드 사제
 Mirror matchup</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>38.06%</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>50.38%</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>언데드 사제</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>59.07%</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>41.85%</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>49.43%</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>34.83%</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>51.65%</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>65.86%</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>64.54%</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>58.04%</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>50.58%</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>34.45%</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>51.46%</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>61.93%</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>사냥개 사냥꾼
-Mirror matchup</t>
-        </is>
-      </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>53.43%</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>사냥개 사냥꾼</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>47.04%</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>36.08%</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>55.83%</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>42.10%</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>40.08%</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>68.53%</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>52.30%</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>44.82%</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>42.20%</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>44.78%</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>35.71%</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>49.61%</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>46.56%</t>
-        </is>
-      </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>Mining Warlock
-Mirror matchup</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Mining Warlock</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
17th commit : 최종 수정 2
</commit_message>
<xml_diff>
--- a/hs_meta.xlsx
+++ b/hs_meta.xlsx
@@ -425,7 +425,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>기간 : LAST_7_DAYS, 대상 : DIAMOND 서버의 REGION_KR 등급 유저</t>
+          <t>기간 : LAST_7_DAYS, 대상 : PLATINUM 서버의 REGION_KR 등급 유저</t>
         </is>
       </c>
     </row>
@@ -464,22 +464,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Plague Death Knight</t>
+          <t>부정 죽음의 기사</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>53.2%</t>
+          <t>31.9%</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>6.5%</t>
+          <t>9.2%</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>34,000</t>
+          <t>15,000</t>
         </is>
       </c>
     </row>
@@ -491,22 +491,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>혈기 죽음의 기사</t>
+          <t>Plague Death Knight</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>49.4%</t>
+          <t>54.8%</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>5.2%</t>
+          <t>6.2%</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>27,000</t>
+          <t>10,000</t>
         </is>
       </c>
     </row>
@@ -518,22 +518,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>부정 죽음의 기사</t>
+          <t>혈기 죽음의 기사</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>25.7%</t>
+          <t>50.9%</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>4.3%</t>
+          <t>3.4%</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>22,000</t>
+          <t>5,600</t>
         </is>
       </c>
     </row>
@@ -545,12 +545,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Highlander Blood Death Knight</t>
+          <t>Rainbow Death Knight</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>51.6%</t>
+          <t>45.8%</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -560,7 +560,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2,400</t>
+          <t>810</t>
         </is>
       </c>
     </row>
@@ -572,22 +572,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Rainbow Death Knight</t>
+          <t>Highlander Blood Death Knight</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>46.0%</t>
+          <t>57.5%</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.4%</t>
+          <t>0.5%</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2,000</t>
+          <t>780</t>
         </is>
       </c>
     </row>
@@ -604,17 +604,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>48.2%</t>
+          <t>43.6%</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.3%</t>
+          <t>0.4%</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1,400</t>
+          <t>700</t>
         </is>
       </c>
     </row>
@@ -631,17 +631,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>39.6%</t>
+          <t>43.8%</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.6%</t>
+          <t>0.7%</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2,900</t>
+          <t>1,200</t>
         </is>
       </c>
     </row>
@@ -658,17 +658,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>50.6%</t>
+          <t>55.3%</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.3%</t>
+          <t>2.5%</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>6,700</t>
+          <t>4,200</t>
         </is>
       </c>
     </row>
@@ -685,7 +685,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>46.0%</t>
+          <t>49.8%</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -695,7 +695,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1,100</t>
+          <t>290</t>
         </is>
       </c>
     </row>
@@ -712,17 +712,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>44.3%</t>
+          <t>32.6%</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.09%</t>
+          <t>0.08%</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>470</t>
+          <t>130</t>
         </is>
       </c>
     </row>
@@ -739,17 +739,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>44.1%</t>
+          <t>36.8%</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.07%</t>
+          <t>0.05%</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>380</t>
+          <t>87</t>
         </is>
       </c>
     </row>
@@ -766,17 +766,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>13.7%</t>
+          <t>15.8%</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.7%</t>
+          <t>0.3%</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>3,700</t>
+          <t>420</t>
         </is>
       </c>
     </row>
@@ -793,17 +793,17 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>56.4%</t>
+          <t>61.7%</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>10.3%</t>
+          <t>7.4%</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>54,000</t>
+          <t>12,000</t>
         </is>
       </c>
     </row>
@@ -820,17 +820,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>52.6%</t>
+          <t>55.2%</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>4.1%</t>
+          <t>3.9%</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>21,000</t>
+          <t>6,500</t>
         </is>
       </c>
     </row>
@@ -847,17 +847,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>54.4%</t>
+          <t>55.6%</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.4%</t>
+          <t>0.9%</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>7,400</t>
+          <t>1,400</t>
         </is>
       </c>
     </row>
@@ -874,7 +874,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>38.0%</t>
+          <t>34.8%</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -884,7 +884,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>3,900</t>
+          <t>1,300</t>
         </is>
       </c>
     </row>
@@ -896,22 +896,22 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>하이랜더 사냥꾼</t>
+          <t>사냥개 사냥꾼</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>59.3%</t>
+          <t>58.9%</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.7%</t>
+          <t>1.8%</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>8,900</t>
+          <t>2,900</t>
         </is>
       </c>
     </row>
@@ -923,22 +923,22 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>사냥개 사냥꾼</t>
+          <t>하이랜더 사냥꾼</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>53.6%</t>
+          <t>61.6%</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.5%</t>
+          <t>1.2%</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>8,000</t>
+          <t>1,900</t>
         </is>
       </c>
     </row>
@@ -955,17 +955,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>56.8%</t>
+          <t>58.2%</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0.4%</t>
+          <t>0.6%</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2,100</t>
+          <t>960</t>
         </is>
       </c>
     </row>
@@ -982,17 +982,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>42.2%</t>
+          <t>39.4%</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.5%</t>
+          <t>0.6%</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2,600</t>
+          <t>1,000</t>
         </is>
       </c>
     </row>
@@ -1009,17 +1009,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>54.6%</t>
+          <t>57.9%</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>13.7%</t>
+          <t>8.4%</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>72,000</t>
+          <t>14,000</t>
         </is>
       </c>
     </row>
@@ -1036,17 +1036,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>49.6%</t>
+          <t>54.0%</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>3.4%</t>
+          <t>3.7%</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>17,000</t>
+          <t>6,100</t>
         </is>
       </c>
     </row>
@@ -1063,17 +1063,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>53.8%</t>
+          <t>62.0%</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.9%</t>
+          <t>1.1%</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>4,700</t>
+          <t>1,900</t>
         </is>
       </c>
     </row>
@@ -1090,17 +1090,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>48.5%</t>
+          <t>55.9%</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0.2%</t>
+          <t>0.4%</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1,200</t>
+          <t>580</t>
         </is>
       </c>
     </row>
@@ -1112,49 +1112,49 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>기타</t>
+          <t>정령 마법사</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>41.4%</t>
+          <t>45.7%</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0.5%</t>
+          <t>0.2%</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2,400</t>
+          <t>310</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>성기사</t>
+          <t>마법사</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>어그로 성기사</t>
+          <t>기타</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>57.5%</t>
+          <t>23.6%</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>5.0%</t>
+          <t>1.2%</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>26,000</t>
+          <t>2,000</t>
         </is>
       </c>
     </row>
@@ -1166,22 +1166,22 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Showdown Paladin</t>
+          <t>어그로 성기사</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>56.5%</t>
+          <t>61.4%</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2.6%</t>
+          <t>5.1%</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>13,000</t>
+          <t>8,600</t>
         </is>
       </c>
     </row>
@@ -1193,22 +1193,22 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>하이랜더 성기사</t>
+          <t>Showdown Paladin</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>53.4%</t>
+          <t>60.3%</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2.5%</t>
+          <t>3.3%</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>13,000</t>
+          <t>5,600</t>
         </is>
       </c>
     </row>
@@ -1220,22 +1220,22 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Earthen Paladin</t>
+          <t>하이랜더 성기사</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>59.0%</t>
+          <t>57.4%</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.0%</t>
+          <t>2.0%</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>5,300</t>
+          <t>3,400</t>
         </is>
       </c>
     </row>
@@ -1252,7 +1252,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>49.4%</t>
+          <t>52.3%</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1262,7 +1262,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1,000</t>
+          <t>380</t>
         </is>
       </c>
     </row>
@@ -1274,49 +1274,49 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>기타</t>
+          <t>Earthen Paladin</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>38.3%</t>
+          <t>53.0%</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.7%</t>
+          <t>0.2%</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>3,400</t>
+          <t>310</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>사제</t>
+          <t>성기사</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>컨트롤 사제</t>
+          <t>기타</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>47.4%</t>
+          <t>40.1%</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>3.3%</t>
+          <t>1.0%</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>17,000</t>
+          <t>1,600</t>
         </is>
       </c>
     </row>
@@ -1328,22 +1328,22 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>언데드 사제</t>
+          <t>컨트롤 사제</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>49.7%</t>
+          <t>50.5%</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1.1%</t>
+          <t>3.5%</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>5,700</t>
+          <t>5,800</t>
         </is>
       </c>
     </row>
@@ -1355,22 +1355,22 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>하이랜더 사제</t>
+          <t>언데드 사제</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>44.7%</t>
+          <t>53.8%</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.4%</t>
+          <t>1.4%</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2,100</t>
+          <t>2,300</t>
         </is>
       </c>
     </row>
@@ -1382,22 +1382,22 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Automaton Priest</t>
+          <t>하이랜더 사제</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>47.0%</t>
+          <t>47.9%</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.3%</t>
+          <t>0.4%</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1,400</t>
+          <t>680</t>
         </is>
       </c>
     </row>
@@ -1409,22 +1409,22 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Ogre Priest</t>
+          <t>Automaton Priest</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>42.7%</t>
+          <t>50.6%</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>0.06%</t>
+          <t>0.2%</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>290</t>
+          <t>320</t>
         </is>
       </c>
     </row>
@@ -1441,17 +1441,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>41.2%</t>
+          <t>35.6%</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>0.3%</t>
+          <t>0.4%</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>1,600</t>
+          <t>740</t>
         </is>
       </c>
     </row>
@@ -1463,12 +1463,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Big Rogue</t>
+          <t>Wishing Rogue</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>48.9%</t>
+          <t>47.2%</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1478,7 +1478,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>5,900</t>
+          <t>1,700</t>
         </is>
       </c>
     </row>
@@ -1490,12 +1490,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Mech Rogue</t>
+          <t>Big Rogue</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>56.6%</t>
+          <t>53.2%</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1505,7 +1505,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>4,100</t>
+          <t>1,400</t>
         </is>
       </c>
     </row>
@@ -1517,22 +1517,22 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>미라클 도적</t>
+          <t>Mining Rogue</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>44.9%</t>
+          <t>46.0%</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>0.7%</t>
+          <t>0.8%</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>3,500</t>
+          <t>1,200</t>
         </is>
       </c>
     </row>
@@ -1544,22 +1544,22 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Wishing Rogue</t>
+          <t>Mech Rogue</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>44.4%</t>
+          <t>62.9%</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>0.6%</t>
+          <t>0.7%</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>3,300</t>
+          <t>1,000</t>
         </is>
       </c>
     </row>
@@ -1571,12 +1571,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Mining Rogue</t>
+          <t>미라클 도적</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>41.7%</t>
+          <t>47.4%</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1586,7 +1586,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2,800</t>
+          <t>890</t>
         </is>
       </c>
     </row>
@@ -1598,22 +1598,22 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>비밀 도적</t>
+          <t>Ogre Rogue</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>49.8%</t>
+          <t>50.0%</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>0.4%</t>
+          <t>0.5%</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2,300</t>
+          <t>800</t>
         </is>
       </c>
     </row>
@@ -1625,12 +1625,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Ogre Rogue</t>
+          <t>비밀 도적</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>46.0%</t>
+          <t>50.5%</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1640,7 +1640,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1,500</t>
+          <t>540</t>
         </is>
       </c>
     </row>
@@ -1657,17 +1657,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>36.5%</t>
+          <t>35.5%</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0.6%</t>
+          <t>1.0%</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>3,100</t>
+          <t>1,600</t>
         </is>
       </c>
     </row>
@@ -1684,17 +1684,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>55.5%</t>
+          <t>59.0%</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>4.3%</t>
+          <t>3.8%</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>22,000</t>
+          <t>6,400</t>
         </is>
       </c>
     </row>
@@ -1711,17 +1711,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>43.9%</t>
+          <t>54.6%</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0.5%</t>
+          <t>0.4%</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2,700</t>
+          <t>700</t>
         </is>
       </c>
     </row>
@@ -1738,7 +1738,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>49.3%</t>
+          <t>48.6%</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1748,7 +1748,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>1,800</t>
+          <t>440</t>
         </is>
       </c>
     </row>
@@ -1765,7 +1765,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>46.7%</t>
+          <t>53.9%</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1775,7 +1775,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>990</t>
+          <t>390</t>
         </is>
       </c>
     </row>
@@ -1792,17 +1792,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>40.7%</t>
+          <t>31.8%</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>0.3%</t>
+          <t>0.4%</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1,300</t>
+          <t>700</t>
         </is>
       </c>
     </row>
@@ -1814,22 +1814,22 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>하이랜더 흑마법사</t>
+          <t>Mining Warlock</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>47.4%</t>
+          <t>52.5%</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>1.0%</t>
+          <t>1.8%</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>5,100</t>
+          <t>2,900</t>
         </is>
       </c>
     </row>
@@ -1841,22 +1841,22 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Mining Warlock</t>
+          <t>타디우스 흑마법사</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>47.4%</t>
+          <t>51.7%</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>0.9%</t>
+          <t>0.8%</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>4,500</t>
+          <t>1,300</t>
         </is>
       </c>
     </row>
@@ -1873,17 +1873,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>47.8%</t>
+          <t>51.0%</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>0.7%</t>
+          <t>0.8%</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>3,800</t>
+          <t>1,200</t>
         </is>
       </c>
     </row>
@@ -1895,22 +1895,22 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Sludge Warlock</t>
+          <t>하이랜더 흑마법사</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>43.1%</t>
+          <t>48.1%</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>0.5%</t>
+          <t>0.7%</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2,600</t>
+          <t>1,000</t>
         </is>
       </c>
     </row>
@@ -1922,22 +1922,22 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>타디우스 흑마법사</t>
+          <t>Sludge Warlock</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>49.8%</t>
+          <t>44.1%</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>0.5%</t>
+          <t>0.6%</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2,500</t>
+          <t>1,000</t>
         </is>
       </c>
     </row>
@@ -1954,17 +1954,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>43.4%</t>
+          <t>42.1%</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>0.7%</t>
+          <t>1.1%</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>3,500</t>
+          <t>1,700</t>
         </is>
       </c>
     </row>
@@ -1981,17 +1981,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>51.1%</t>
+          <t>54.3%</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>4.1%</t>
+          <t>5.1%</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>21,000</t>
+          <t>8,500</t>
         </is>
       </c>
     </row>
@@ -2008,7 +2008,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>55.7%</t>
+          <t>60.4%</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -2018,7 +2018,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>10,000</t>
+          <t>3,200</t>
         </is>
       </c>
     </row>
@@ -2030,22 +2030,22 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Rock 'n' Roll Warrior</t>
+          <t>하이랜더 전사</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>51.0%</t>
+          <t>47.1%</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>0.8%</t>
+          <t>0.4%</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>4,300</t>
+          <t>690</t>
         </is>
       </c>
     </row>
@@ -2057,22 +2057,22 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>하이랜더 전사</t>
+          <t>Rock 'n' Roll Warrior</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>47.6%</t>
+          <t>52.9%</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>0.5%</t>
+          <t>0.3%</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2,700</t>
+          <t>540</t>
         </is>
       </c>
     </row>
@@ -2089,17 +2089,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>39.7%</t>
+          <t>39.2%</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>0.1%</t>
+          <t>0.2%</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>680</t>
+          <t>310</t>
         </is>
       </c>
     </row>
@@ -2116,17 +2116,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>43.1%</t>
+          <t>29.0%</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>0.4%</t>
+          <t>1.5%</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>2,200</t>
+          <t>2,400</t>
         </is>
       </c>
     </row>
@@ -2152,7 +2152,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>기간 : LAST_7_DAYS, 대상 : DIAMOND 서버의 REGION_KR 등급 유저</t>
+          <t>기간 : LAST_7_DAYS, 대상 : PLATINUM 서버의 REGION_KR 등급 유저</t>
         </is>
       </c>
     </row>
@@ -2160,59 +2160,59 @@
       <c r="A2" t="inlineStr"/>
       <c r="B2" t="inlineStr">
         <is>
+          <t>부정 죽음의 기사</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>Rainbow Mage</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>용 드루이드</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>Plague Death Knight</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>어그로 성기사</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>컨트롤 전사</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>하이랜더 드루이드</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>하이랜더 주술사</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Mining Mage</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>컨트롤 사제</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
         <is>
           <t>혈기 죽음의 기사</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>어그로 성기사</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>하이랜더 주술사</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>부정 죽음의 기사</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>하이랜더 드루이드</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>컨트롤 전사</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Mining Mage</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>컨트롤 사제</t>
-        </is>
-      </c>
       <c r="M2" t="inlineStr">
         <is>
           <t>Showdown Paladin</t>
@@ -2220,12 +2220,12 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
+          <t>어그로 악마사냥꾼</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
           <t>하이랜더 성기사</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>격노 전사</t>
         </is>
       </c>
       <c r="P2" t="inlineStr"/>
@@ -2242,858 +2242,858 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>부정 죽음의 기사</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>부정 죽음의 기사
+Mirror matchup</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>21.23%</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>16.51%</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>28.88%</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>32.19%</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>26.34%</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>30.00%</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>17.92%</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>28.71%</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>30.42%</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>28.51%</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>24.35%</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>40.62%</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>20.14%</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>Rainbow Mage</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>78.76%</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
         <is>
           <t>Rainbow Mage
 Mirror matchup</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>44.87%</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>55.54%</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>54.07%</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>50.80%</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>51.99%</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>76.81%</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>48.62%</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>53.70%</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>58.56%</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>67.43%</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>53.45%</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>55.28%</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>40.85%</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>44.40%</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>58.59%</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>50.24%</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>49.23%</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>47.68%</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>58.20%</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>62.34%</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>65.28%</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>57.24%</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>43.96%</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>52.68%</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>54.92%</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
         <is>
           <t>용 드루이드</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>55.12%</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>83.48%</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>55.59%</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>용 드루이드
 Mirror matchup</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>60.76%</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>57.04%</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>35.54%</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>48.20%</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>85.07%</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>46.35%</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>57.31%</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>65.71%</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>50.22%</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>35.03%</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>38.15%</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>63.82%</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>54.71%</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>35.35%</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>58.57%</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>50.00%</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>44.05%</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>64.33%</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>50.46%</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>69.86%</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>44.95%</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>65.06%</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>40.62%</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
         <is>
           <t>Plague Death Knight</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>44.45%</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>39.23%</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>71.11%</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>41.40%</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>45.28%</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
         <is>
           <t>Plague Death Knight
 Mirror matchup</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>56.64%</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>42.56%</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>40.90%</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>55.42%</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>60.60%</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>65.69%</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>44.69%</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>55.73%</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
         <is>
           <t>64.53%</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>73.27%</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>59.56%</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>59.81%</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>49.26%</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>60.52%</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>50.06%</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>62.63%</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>42.47%</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>47.54%</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>47.05%</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>57.14%</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>어그로 성기사</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>67.80%</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>49.75%</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>64.64%</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>59.09%</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>어그로 성기사
+Mirror matchup</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>58.46%</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>64.91%</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>52.74%</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>48.64%</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>60.16%</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>68.38%</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>42.85%</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>47.42%</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>57.97%</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>컨트롤 전사</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>73.65%</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>50.76%</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>41.42%</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>44.57%</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>41.53%</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>컨트롤 전사
+Mirror matchup</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>38.61%</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>53.19%</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>54.23%</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>50.00%</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>53.33%</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>43.08%</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>45.36%</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>55.22%</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>하이랜더 드루이드</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>70.00%</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>52.31%</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>50.00%</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>39.39%</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>35.08%</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>61.38%</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>하이랜더 드루이드
+Mirror matchup</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>33.33%</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>57.97%</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>66.66%</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>61.33%</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>46.25%</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>38.09%</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>30.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>하이랜더 주술사</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>82.07%</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>41.79%</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>55.94%</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>34.30%</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>47.25%</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>46.80%</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>66.66%</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>하이랜더 주술사
+Mirror matchup</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>50.00%</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>61.42%</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>64.06%</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>63.07%</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>48.64%</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>64.44%</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Mining Mage</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>71.28%</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>37.65%</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>35.66%</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>55.30%</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>51.35%</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>45.76%</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>42.02%</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>50.00%</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Mining Mage
+Mirror matchup</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>71.66%</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>69.69%</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>52.05%</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>39.68%</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>45.71%</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>컨트롤 사제</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>69.57%</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>34.71%</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>49.53%</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>44.26%</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>39.83%</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>49.05%</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>33.33%</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>38.57%</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>28.33%</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>컨트롤 사제
+Mirror matchup</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>66.15%</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>48.78%</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>36.17%</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>29.78%</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
         <is>
           <t>혈기 죽음의 기사</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>45.92%</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>42.95%</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>43.35%</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>71.48%</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>42.75%</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>30.13%</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>35.46%</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>31.61%</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>45.83%</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>38.66%</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>35.93%</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>30.30%</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>33.84%</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
         <is>
           <t>혈기 죽음의 기사
 Mirror matchup</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>47.26%</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>43.10%</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>75.27%</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>44.67%</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>43.22%</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>47.55%</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>52.43%</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>53.30%</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>48.42%</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>42.51%</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>어그로 성기사</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>49.19%</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>64.45%</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>57.43%</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>52.73%</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>어그로 성기사
-Mirror matchup</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>49.22%</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>74.21%</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>67.46%</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>51.82%</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>49.23%</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>54.58%</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>42.56%</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>56.16%</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>39.06%</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>하이랜더 주술사</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>48.00%</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>51.79%</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>35.46%</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>56.89%</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>50.77%</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>하이랜더 주술사
-Mirror matchup</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>84.43%</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>56.19%</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>50.38%</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>54.57%</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>62.47%</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>53.62%</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>60.39%</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>56.31%</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>부정 죽음의 기사</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>23.18%</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>14.92%</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>26.72%</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>24.72%</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>25.78%</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>15.56%</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>부정 죽음의 기사
-Mirror matchup</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>28.53%</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>21.70%</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>24.96%</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>22.79%</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>19.10%</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>18.25%</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>20.85%</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>하이랜더 드루이드</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>51.37%</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>53.64%</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>40.43%</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>55.32%</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>32.53%</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>43.80%</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>71.46%</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>하이랜더 드루이드
-Mirror matchup</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>62.89%</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>62.71%</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>57.22%</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>36.38%</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>42.71%</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>54.34%</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>컨트롤 전사</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>46.29%</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>42.68%</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>40.18%</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>56.77%</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>48.17%</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>49.61%</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>78.29%</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>37.10%</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>컨트롤 전사
-Mirror matchup</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>48.25%</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>55.30%</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>53.68%</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>50.97%</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>51.62%</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Mining Mage</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>41.43%</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>34.28%</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>50.73%</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>52.44%</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>50.76%</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>45.42%</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>75.03%</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>37.28%</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>51.74%</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>Mining Mage
-Mirror matchup</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>66.81%</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>49.29%</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>48.26%</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>31.74%</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>컨트롤 사제</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>32.56%</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>49.77%</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>39.47%</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>47.56%</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>45.41%</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>37.34%</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>77.20%</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>42.77%</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>44.69%</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>33.18%</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>컨트롤 사제
-Mirror matchup</t>
-        </is>
-      </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>49.11%</t>
+          <t>35.06%</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>40.13%</t>
+          <t>44.64%</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>51.79%</t>
+          <t>44.68%</t>
         </is>
       </c>
     </row>
@@ -3105,57 +3105,57 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>46.54%</t>
+          <t>75.64%</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>64.96%</t>
+          <t>56.03%</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>49.93%</t>
+          <t>55.04%</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>46.69%</t>
+          <t>52.45%</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>57.43%</t>
+          <t>57.14%</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>46.37%</t>
+          <t>56.91%</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>80.89%</t>
+          <t>53.75%</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>63.61%</t>
+          <t>36.92%</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>46.31%</t>
+          <t>47.94%</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>50.70%</t>
+          <t>51.21%</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>50.88%</t>
+          <t>64.93%</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
@@ -3166,167 +3166,169 @@
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>50.34%</t>
+          <t>56.36%</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>39.39%</t>
+          <t>50.72%</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>하이랜더 성기사</t>
+          <t>어그로 악마사냥꾼</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>44.71%</t>
+          <t>59.37%</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>61.84%</t>
+          <t>47.31%</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>37.36%</t>
+          <t>34.93%</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>51.57%</t>
+          <t>52.94%</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>43.83%</t>
+          <t>52.57%</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>39.60%</t>
+          <t>54.63%</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>81.74%</t>
+          <t>61.90%</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>57.28%</t>
+          <t>51.35%</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>49.02%</t>
+          <t>60.31%</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>51.73%</t>
+          <t>63.82%</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>59.86%</t>
+          <t>55.35%</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>49.65%</t>
+          <t>43.63%</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>하이랜더 성기사
+          <t>어그로 악마사냥꾼
 Mirror matchup</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>46.90%</t>
+          <t>Not enough games
+⁓</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>격노 전사</t>
+          <t>하이랜더 성기사</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>59.14%</t>
+          <t>79.85%</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>36.17%</t>
+          <t>45.07%</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>57.52%</t>
+          <t>59.37%</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>57.48%</t>
+          <t>42.85%</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>60.93%</t>
+          <t>42.02%</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>43.68%</t>
+          <t>44.77%</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>79.14%</t>
+          <t>70.00%</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>45.65%</t>
+          <t>35.55%</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>48.37%</t>
+          <t>54.28%</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>68.25%</t>
+          <t>70.21%</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>48.20%</t>
+          <t>55.31%</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>60.60%</t>
+          <t>49.27%</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>53.09%</t>
+          <t>Not enough games
+⁓</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>격노 전사
+          <t>하이랜더 성기사
 Mirror matchup</t>
         </is>
       </c>

</xml_diff>